<commit_message>
Add pre-final version for short report, report
</commit_message>
<xml_diff>
--- a/Other/Tmp/Tasksheet Final.xlsx
+++ b/Other/Tmp/Tasksheet Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phongbv\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everything\Desktop\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="134">
   <si>
     <t>No.</t>
   </si>
@@ -759,6 +759,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,15 +782,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1090,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C74" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85:J85"/>
+    <sheetView tabSelected="1" topLeftCell="C91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J122" sqref="J122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1135,10 +1135,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="32">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -1155,8 +1155,8 @@
       <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="4" t="s">
         <v>41</v>
       </c>
@@ -1171,8 +1171,8 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="4" t="s">
         <v>82</v>
       </c>
@@ -1187,8 +1187,8 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="4" t="s">
         <v>42</v>
       </c>
@@ -1203,8 +1203,8 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1219,8 +1219,8 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
@@ -1235,10 +1235,10 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="33">
+      <c r="A8" s="29">
         <v>2</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1255,8 +1255,8 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1271,8 +1271,8 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1287,8 +1287,8 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" ht="15.75">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1303,10 +1303,10 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="33">
+      <c r="A12" s="29">
         <v>3</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1323,8 +1323,8 @@
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1337,8 +1337,8 @@
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="22" t="s">
         <v>14</v>
       </c>
@@ -1353,8 +1353,8 @@
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="23" t="s">
         <v>15</v>
       </c>
@@ -1367,14 +1367,15 @@
       <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>83</v>
       </c>
+      <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -1382,14 +1383,15 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>83</v>
       </c>
+      <c r="E17" s="20"/>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -1397,14 +1399,15 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="19" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>83</v>
       </c>
+      <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -1412,8 +1415,8 @@
       <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="19" t="s">
         <v>57</v>
       </c>
@@ -1428,8 +1431,8 @@
       <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="19" t="s">
         <v>47</v>
       </c>
@@ -1444,8 +1447,8 @@
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="23" t="s">
         <v>16</v>
       </c>
@@ -1458,14 +1461,15 @@
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>83</v>
       </c>
+      <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -1473,8 +1477,8 @@
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="19" t="s">
         <v>18</v>
       </c>
@@ -1489,8 +1493,8 @@
       <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="19" t="s">
         <v>48</v>
       </c>
@@ -1505,8 +1509,8 @@
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="19" t="s">
         <v>102</v>
       </c>
@@ -1521,14 +1525,15 @@
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>83</v>
       </c>
+      <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -1536,8 +1541,8 @@
       <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="7" t="s">
         <v>50</v>
       </c>
@@ -1552,8 +1557,8 @@
       <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="7" t="s">
         <v>53</v>
       </c>
@@ -1568,8 +1573,8 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1586,8 +1591,8 @@
       <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="4" t="s">
         <v>52</v>
       </c>
@@ -1602,8 +1607,8 @@
       <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="1" t="s">
         <v>20</v>
       </c>
@@ -1618,8 +1623,8 @@
       <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="4" t="s">
         <v>28</v>
       </c>
@@ -1634,8 +1639,8 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="5" t="s">
         <v>103</v>
       </c>
@@ -1648,8 +1653,8 @@
       <c r="J33" s="21"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="19" t="s">
         <v>105</v>
       </c>
@@ -1664,8 +1669,8 @@
       <c r="J34" s="21"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="19" t="s">
         <v>104</v>
       </c>
@@ -1680,8 +1685,8 @@
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="19" t="s">
         <v>106</v>
       </c>
@@ -1696,8 +1701,8 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="19" t="s">
         <v>107</v>
       </c>
@@ -1712,8 +1717,8 @@
       <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="19" t="s">
         <v>108</v>
       </c>
@@ -1728,8 +1733,8 @@
       <c r="J38" s="21"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="19" t="s">
         <v>109</v>
       </c>
@@ -1744,8 +1749,8 @@
       <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="19" t="s">
         <v>110</v>
       </c>
@@ -1760,8 +1765,8 @@
       <c r="J40" s="21"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="18" t="s">
         <v>21</v>
       </c>
@@ -1774,8 +1779,8 @@
       <c r="J41" s="21"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="19" t="s">
         <v>60</v>
       </c>
@@ -1790,8 +1795,8 @@
       <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="19" t="s">
         <v>84</v>
       </c>
@@ -1806,8 +1811,8 @@
       <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="19" t="s">
         <v>85</v>
       </c>
@@ -1822,8 +1827,8 @@
       <c r="J44" s="21"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="19" t="s">
         <v>86</v>
       </c>
@@ -1838,8 +1843,8 @@
       <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="24" t="s">
         <v>87</v>
       </c>
@@ -1854,8 +1859,8 @@
       <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="5" t="s">
         <v>54</v>
       </c>
@@ -1868,8 +1873,8 @@
       <c r="J47" s="21"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="19" t="s">
         <v>19</v>
       </c>
@@ -1884,8 +1889,8 @@
       <c r="J48" s="21"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="19" t="s">
         <v>53</v>
       </c>
@@ -1900,8 +1905,8 @@
       <c r="J49" s="21"/>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="18" t="s">
         <v>27</v>
       </c>
@@ -1914,8 +1919,8 @@
       <c r="J50" s="21"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
       <c r="C51" s="19" t="s">
         <v>61</v>
       </c>
@@ -1930,8 +1935,8 @@
       <c r="J51" s="21"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="31"/>
-      <c r="B52" s="31"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="34"/>
       <c r="C52" s="19" t="s">
         <v>63</v>
       </c>
@@ -1946,8 +1951,8 @@
       <c r="J52" s="21"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="32"/>
-      <c r="B53" s="32"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="24" t="s">
         <v>111</v>
       </c>
@@ -1962,10 +1967,10 @@
       <c r="J53" s="21"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="27">
+      <c r="A54" s="30">
         <v>5</v>
       </c>
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C54" s="5" t="s">
@@ -1980,8 +1985,8 @@
       <c r="J54" s="21"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="28"/>
-      <c r="B55" s="33"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="29"/>
       <c r="C55" s="6" t="s">
         <v>98</v>
       </c>
@@ -1996,8 +2001,8 @@
       <c r="J55" s="21"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="28"/>
-      <c r="B56" s="33"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="6" t="s">
         <v>67</v>
       </c>
@@ -2012,8 +2017,8 @@
       <c r="J56" s="21"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="28"/>
-      <c r="B57" s="33"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="5" t="s">
         <v>64</v>
       </c>
@@ -2026,8 +2031,8 @@
       <c r="J57" s="21"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="28"/>
-      <c r="B58" s="33"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="6" t="s">
         <v>65</v>
       </c>
@@ -2044,8 +2049,8 @@
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="28"/>
-      <c r="B59" s="33"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="6" t="s">
         <v>66</v>
       </c>
@@ -2062,8 +2067,8 @@
       </c>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="28"/>
-      <c r="B60" s="33"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="5" t="s">
         <v>55</v>
       </c>
@@ -2076,8 +2081,8 @@
       <c r="J60" s="21"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="28"/>
-      <c r="B61" s="33"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="29"/>
       <c r="C61" s="6" t="s">
         <v>58</v>
       </c>
@@ -2094,8 +2099,8 @@
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="28"/>
-      <c r="B62" s="33"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="29"/>
       <c r="C62" s="6" t="s">
         <v>56</v>
       </c>
@@ -2112,8 +2117,8 @@
       </c>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="28"/>
-      <c r="B63" s="33"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="29"/>
       <c r="C63" s="6" t="s">
         <v>89</v>
       </c>
@@ -2130,8 +2135,8 @@
       </c>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="28"/>
-      <c r="B64" s="33"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="29"/>
       <c r="C64" s="6" t="s">
         <v>90</v>
       </c>
@@ -2148,9 +2153,9 @@
       </c>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="28"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="34" t="s">
+      <c r="A65" s="31"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="27" t="s">
         <v>69</v>
       </c>
       <c r="D65" s="20"/>
@@ -2162,8 +2167,8 @@
       <c r="J65" s="21"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="28"/>
-      <c r="B66" s="33"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="29"/>
       <c r="C66" s="19" t="s">
         <v>112</v>
       </c>
@@ -2180,8 +2185,8 @@
       </c>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="28"/>
-      <c r="B67" s="33"/>
+      <c r="A67" s="31"/>
+      <c r="B67" s="29"/>
       <c r="C67" s="19" t="s">
         <v>113</v>
       </c>
@@ -2198,9 +2203,9 @@
       </c>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="28"/>
-      <c r="B68" s="33"/>
-      <c r="C68" s="34" t="s">
+      <c r="A68" s="31"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="27" t="s">
         <v>70</v>
       </c>
       <c r="D68" s="20"/>
@@ -2212,8 +2217,8 @@
       <c r="J68" s="21"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="28"/>
-      <c r="B69" s="33"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="29"/>
       <c r="C69" s="19" t="s">
         <v>114</v>
       </c>
@@ -2230,8 +2235,8 @@
       </c>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="28"/>
-      <c r="B70" s="33"/>
+      <c r="A70" s="31"/>
+      <c r="B70" s="29"/>
       <c r="C70" s="6" t="s">
         <v>91</v>
       </c>
@@ -2248,9 +2253,9 @@
       </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="28"/>
-      <c r="B71" s="33"/>
-      <c r="C71" s="34" t="s">
+      <c r="A71" s="31"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="27" t="s">
         <v>92</v>
       </c>
       <c r="D71" s="20"/>
@@ -2262,8 +2267,8 @@
       <c r="J71" s="21"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="28"/>
-      <c r="B72" s="33"/>
+      <c r="A72" s="31"/>
+      <c r="B72" s="29"/>
       <c r="C72" s="19" t="s">
         <v>115</v>
       </c>
@@ -2280,8 +2285,8 @@
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="28"/>
-      <c r="B73" s="33"/>
+      <c r="A73" s="31"/>
+      <c r="B73" s="29"/>
       <c r="C73" s="19" t="s">
         <v>116</v>
       </c>
@@ -2298,8 +2303,8 @@
       </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="28"/>
-      <c r="B74" s="33"/>
+      <c r="A74" s="31"/>
+      <c r="B74" s="29"/>
       <c r="C74" s="6" t="s">
         <v>93</v>
       </c>
@@ -2312,8 +2317,8 @@
       <c r="J74" s="21"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="28"/>
-      <c r="B75" s="33"/>
+      <c r="A75" s="31"/>
+      <c r="B75" s="29"/>
       <c r="C75" s="19" t="s">
         <v>118</v>
       </c>
@@ -2330,8 +2335,8 @@
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="28"/>
-      <c r="B76" s="33"/>
+      <c r="A76" s="31"/>
+      <c r="B76" s="29"/>
       <c r="C76" s="19" t="s">
         <v>117</v>
       </c>
@@ -2348,8 +2353,8 @@
       </c>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="28"/>
-      <c r="B77" s="33"/>
+      <c r="A77" s="31"/>
+      <c r="B77" s="29"/>
       <c r="C77" s="6" t="s">
         <v>101</v>
       </c>
@@ -2366,8 +2371,8 @@
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="28"/>
-      <c r="B78" s="33"/>
+      <c r="A78" s="31"/>
+      <c r="B78" s="29"/>
       <c r="C78" s="5" t="s">
         <v>68</v>
       </c>
@@ -2380,8 +2385,8 @@
       <c r="J78" s="21"/>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="28"/>
-      <c r="B79" s="33"/>
+      <c r="A79" s="31"/>
+      <c r="B79" s="29"/>
       <c r="C79" s="6" t="s">
         <v>58</v>
       </c>
@@ -2398,8 +2403,8 @@
       </c>
     </row>
     <row r="80" spans="1:10">
-      <c r="A80" s="28"/>
-      <c r="B80" s="33"/>
+      <c r="A80" s="31"/>
+      <c r="B80" s="29"/>
       <c r="C80" s="6" t="s">
         <v>100</v>
       </c>
@@ -2416,9 +2421,9 @@
       </c>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="28"/>
-      <c r="B81" s="33"/>
-      <c r="C81" s="34" t="s">
+      <c r="A81" s="31"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="27" t="s">
         <v>69</v>
       </c>
       <c r="D81" s="20"/>
@@ -2430,8 +2435,8 @@
       <c r="J81" s="21"/>
     </row>
     <row r="82" spans="1:10">
-      <c r="A82" s="28"/>
-      <c r="B82" s="33"/>
+      <c r="A82" s="31"/>
+      <c r="B82" s="29"/>
       <c r="C82" s="19" t="s">
         <v>112</v>
       </c>
@@ -2448,8 +2453,8 @@
       </c>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="28"/>
-      <c r="B83" s="33"/>
+      <c r="A83" s="31"/>
+      <c r="B83" s="29"/>
       <c r="C83" s="19" t="s">
         <v>113</v>
       </c>
@@ -2466,9 +2471,9 @@
       </c>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="28"/>
-      <c r="B84" s="33"/>
-      <c r="C84" s="34" t="s">
+      <c r="A84" s="31"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="27" t="s">
         <v>70</v>
       </c>
       <c r="D84" s="20"/>
@@ -2480,8 +2485,8 @@
       <c r="J84" s="21"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="28"/>
-      <c r="B85" s="33"/>
+      <c r="A85" s="31"/>
+      <c r="B85" s="29"/>
       <c r="C85" s="19" t="s">
         <v>114</v>
       </c>
@@ -2498,8 +2503,8 @@
       </c>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="28"/>
-      <c r="B86" s="33"/>
+      <c r="A86" s="31"/>
+      <c r="B86" s="29"/>
       <c r="C86" s="6" t="s">
         <v>91</v>
       </c>
@@ -2516,9 +2521,9 @@
       </c>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="28"/>
-      <c r="B87" s="33"/>
-      <c r="C87" s="34" t="s">
+      <c r="A87" s="31"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="27" t="s">
         <v>92</v>
       </c>
       <c r="D87" s="20"/>
@@ -2530,8 +2535,8 @@
       <c r="J87" s="21"/>
     </row>
     <row r="88" spans="1:10">
-      <c r="A88" s="28"/>
-      <c r="B88" s="33"/>
+      <c r="A88" s="31"/>
+      <c r="B88" s="29"/>
       <c r="C88" s="19" t="s">
         <v>115</v>
       </c>
@@ -2548,8 +2553,8 @@
       </c>
     </row>
     <row r="89" spans="1:10">
-      <c r="A89" s="28"/>
-      <c r="B89" s="33"/>
+      <c r="A89" s="31"/>
+      <c r="B89" s="29"/>
       <c r="C89" s="19" t="s">
         <v>116</v>
       </c>
@@ -2566,8 +2571,8 @@
       </c>
     </row>
     <row r="90" spans="1:10">
-      <c r="A90" s="28"/>
-      <c r="B90" s="33"/>
+      <c r="A90" s="31"/>
+      <c r="B90" s="29"/>
       <c r="C90" s="6" t="s">
         <v>101</v>
       </c>
@@ -2584,8 +2589,8 @@
       </c>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="28"/>
-      <c r="B91" s="33"/>
+      <c r="A91" s="31"/>
+      <c r="B91" s="29"/>
       <c r="C91" s="6" t="s">
         <v>87</v>
       </c>
@@ -2602,8 +2607,8 @@
       </c>
     </row>
     <row r="92" spans="1:10">
-      <c r="A92" s="28"/>
-      <c r="B92" s="33"/>
+      <c r="A92" s="31"/>
+      <c r="B92" s="29"/>
       <c r="C92" s="6" t="s">
         <v>86</v>
       </c>
@@ -2620,9 +2625,9 @@
       </c>
     </row>
     <row r="93" spans="1:10">
-      <c r="A93" s="28"/>
-      <c r="B93" s="33"/>
-      <c r="C93" s="34" t="s">
+      <c r="A93" s="31"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D93" s="20"/>
@@ -2634,8 +2639,8 @@
       <c r="J93" s="21"/>
     </row>
     <row r="94" spans="1:10">
-      <c r="A94" s="28"/>
-      <c r="B94" s="33"/>
+      <c r="A94" s="31"/>
+      <c r="B94" s="29"/>
       <c r="C94" s="19" t="s">
         <v>119</v>
       </c>
@@ -2652,8 +2657,8 @@
       </c>
     </row>
     <row r="95" spans="1:10">
-      <c r="A95" s="28"/>
-      <c r="B95" s="33"/>
+      <c r="A95" s="31"/>
+      <c r="B95" s="29"/>
       <c r="C95" s="19" t="s">
         <v>133</v>
       </c>
@@ -2670,9 +2675,9 @@
       </c>
     </row>
     <row r="96" spans="1:10">
-      <c r="A96" s="28"/>
-      <c r="B96" s="33"/>
-      <c r="C96" s="34" t="s">
+      <c r="A96" s="31"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="27" t="s">
         <v>95</v>
       </c>
       <c r="D96" s="20"/>
@@ -2686,8 +2691,8 @@
       <c r="J96" s="21"/>
     </row>
     <row r="97" spans="1:10">
-      <c r="A97" s="28"/>
-      <c r="B97" s="33"/>
+      <c r="A97" s="31"/>
+      <c r="B97" s="29"/>
       <c r="C97" s="19" t="s">
         <v>120</v>
       </c>
@@ -2702,9 +2707,9 @@
       </c>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="28"/>
-      <c r="B98" s="33"/>
-      <c r="C98" s="34" t="s">
+      <c r="A98" s="31"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="27" t="s">
         <v>99</v>
       </c>
       <c r="D98" s="20"/>
@@ -2716,8 +2721,8 @@
       <c r="J98" s="21"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="28"/>
-      <c r="B99" s="33"/>
+      <c r="A99" s="31"/>
+      <c r="B99" s="29"/>
       <c r="C99" s="19" t="s">
         <v>121</v>
       </c>
@@ -2734,8 +2739,8 @@
       </c>
     </row>
     <row r="100" spans="1:10">
-      <c r="A100" s="28"/>
-      <c r="B100" s="33"/>
+      <c r="A100" s="31"/>
+      <c r="B100" s="29"/>
       <c r="C100" s="19" t="s">
         <v>122</v>
       </c>
@@ -2752,8 +2757,8 @@
       </c>
     </row>
     <row r="101" spans="1:10">
-      <c r="A101" s="28"/>
-      <c r="B101" s="33"/>
+      <c r="A101" s="31"/>
+      <c r="B101" s="29"/>
       <c r="C101" s="5" t="s">
         <v>67</v>
       </c>
@@ -2766,8 +2771,8 @@
       <c r="J101" s="21"/>
     </row>
     <row r="102" spans="1:10">
-      <c r="A102" s="28"/>
-      <c r="B102" s="33"/>
+      <c r="A102" s="31"/>
+      <c r="B102" s="29"/>
       <c r="C102" s="6" t="s">
         <v>58</v>
       </c>
@@ -2784,8 +2789,8 @@
       </c>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="28"/>
-      <c r="B103" s="33"/>
+      <c r="A103" s="31"/>
+      <c r="B103" s="29"/>
       <c r="C103" s="6" t="s">
         <v>56</v>
       </c>
@@ -2802,9 +2807,9 @@
       </c>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="28"/>
-      <c r="B104" s="33"/>
-      <c r="C104" s="34" t="s">
+      <c r="A104" s="31"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="27" t="s">
         <v>87</v>
       </c>
       <c r="D104" s="20"/>
@@ -2816,8 +2821,8 @@
       <c r="J104" s="21"/>
     </row>
     <row r="105" spans="1:10">
-      <c r="A105" s="28"/>
-      <c r="B105" s="33"/>
+      <c r="A105" s="31"/>
+      <c r="B105" s="29"/>
       <c r="C105" s="19" t="s">
         <v>123</v>
       </c>
@@ -2834,8 +2839,8 @@
       </c>
     </row>
     <row r="106" spans="1:10">
-      <c r="A106" s="28"/>
-      <c r="B106" s="33"/>
+      <c r="A106" s="31"/>
+      <c r="B106" s="29"/>
       <c r="C106" s="19" t="s">
         <v>124</v>
       </c>
@@ -2852,9 +2857,9 @@
       </c>
     </row>
     <row r="107" spans="1:10">
-      <c r="A107" s="28"/>
-      <c r="B107" s="33"/>
-      <c r="C107" s="34" t="s">
+      <c r="A107" s="31"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="27" t="s">
         <v>86</v>
       </c>
       <c r="D107" s="20"/>
@@ -2866,8 +2871,8 @@
       <c r="J107" s="21"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="28"/>
-      <c r="B108" s="33"/>
+      <c r="A108" s="31"/>
+      <c r="B108" s="29"/>
       <c r="C108" s="19" t="s">
         <v>125</v>
       </c>
@@ -2884,8 +2889,8 @@
       </c>
     </row>
     <row r="109" spans="1:10">
-      <c r="A109" s="28"/>
-      <c r="B109" s="33"/>
+      <c r="A109" s="31"/>
+      <c r="B109" s="29"/>
       <c r="C109" s="19" t="s">
         <v>126</v>
       </c>
@@ -2902,8 +2907,8 @@
       </c>
     </row>
     <row r="110" spans="1:10">
-      <c r="A110" s="28"/>
-      <c r="B110" s="33"/>
+      <c r="A110" s="31"/>
+      <c r="B110" s="29"/>
       <c r="C110" s="19" t="s">
         <v>127</v>
       </c>
@@ -2920,8 +2925,8 @@
       </c>
     </row>
     <row r="111" spans="1:10">
-      <c r="A111" s="28"/>
-      <c r="B111" s="33"/>
+      <c r="A111" s="31"/>
+      <c r="B111" s="29"/>
       <c r="C111" s="19" t="s">
         <v>128</v>
       </c>
@@ -2938,8 +2943,8 @@
       </c>
     </row>
     <row r="112" spans="1:10">
-      <c r="A112" s="28"/>
-      <c r="B112" s="33"/>
+      <c r="A112" s="31"/>
+      <c r="B112" s="29"/>
       <c r="C112" s="19" t="s">
         <v>129</v>
       </c>
@@ -2956,9 +2961,9 @@
       </c>
     </row>
     <row r="113" spans="1:10">
-      <c r="A113" s="28"/>
-      <c r="B113" s="33"/>
-      <c r="C113" s="34" t="s">
+      <c r="A113" s="31"/>
+      <c r="B113" s="29"/>
+      <c r="C113" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D113" s="20"/>
@@ -2970,8 +2975,8 @@
       <c r="J113" s="21"/>
     </row>
     <row r="114" spans="1:10">
-      <c r="A114" s="28"/>
-      <c r="B114" s="33"/>
+      <c r="A114" s="31"/>
+      <c r="B114" s="29"/>
       <c r="C114" s="19" t="s">
         <v>130</v>
       </c>
@@ -2988,8 +2993,8 @@
       </c>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="28"/>
-      <c r="B115" s="33"/>
+      <c r="A115" s="31"/>
+      <c r="B115" s="29"/>
       <c r="C115" s="19" t="s">
         <v>111</v>
       </c>
@@ -3006,9 +3011,9 @@
       </c>
     </row>
     <row r="116" spans="1:10">
-      <c r="A116" s="28"/>
-      <c r="B116" s="33"/>
-      <c r="C116" s="34" t="s">
+      <c r="A116" s="31"/>
+      <c r="B116" s="29"/>
+      <c r="C116" s="27" t="s">
         <v>95</v>
       </c>
       <c r="D116" s="20"/>
@@ -3020,8 +3025,8 @@
       <c r="J116" s="21"/>
     </row>
     <row r="117" spans="1:10">
-      <c r="A117" s="28"/>
-      <c r="B117" s="33"/>
+      <c r="A117" s="31"/>
+      <c r="B117" s="29"/>
       <c r="C117" s="19" t="s">
         <v>120</v>
       </c>
@@ -3038,8 +3043,8 @@
       </c>
     </row>
     <row r="118" spans="1:10">
-      <c r="A118" s="28"/>
-      <c r="B118" s="33"/>
+      <c r="A118" s="31"/>
+      <c r="B118" s="29"/>
       <c r="C118" s="6" t="s">
         <v>131</v>
       </c>
@@ -3056,9 +3061,9 @@
       </c>
     </row>
     <row r="119" spans="1:10">
-      <c r="A119" s="28"/>
-      <c r="B119" s="33"/>
-      <c r="C119" s="34" t="s">
+      <c r="A119" s="31"/>
+      <c r="B119" s="29"/>
+      <c r="C119" s="27" t="s">
         <v>99</v>
       </c>
       <c r="D119" s="20"/>
@@ -3070,8 +3075,8 @@
       <c r="J119" s="21"/>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="28"/>
-      <c r="B120" s="33"/>
+      <c r="A120" s="31"/>
+      <c r="B120" s="29"/>
       <c r="C120" s="19" t="s">
         <v>121</v>
       </c>
@@ -3088,8 +3093,8 @@
       </c>
     </row>
     <row r="121" spans="1:10">
-      <c r="A121" s="28"/>
-      <c r="B121" s="33"/>
+      <c r="A121" s="31"/>
+      <c r="B121" s="29"/>
       <c r="C121" s="19" t="s">
         <v>122</v>
       </c>
@@ -3106,13 +3111,15 @@
       </c>
     </row>
     <row r="122" spans="1:10">
-      <c r="A122" s="28"/>
-      <c r="B122" s="33"/>
+      <c r="A122" s="31"/>
+      <c r="B122" s="29"/>
       <c r="C122" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D122" s="20"/>
-      <c r="E122" s="20"/>
+      <c r="E122" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="F122" s="20"/>
       <c r="G122" s="20"/>
       <c r="H122" s="20"/>
@@ -3122,8 +3129,8 @@
       </c>
     </row>
     <row r="123" spans="1:10">
-      <c r="A123" s="28"/>
-      <c r="B123" s="33"/>
+      <c r="A123" s="31"/>
+      <c r="B123" s="29"/>
       <c r="C123" s="4" t="s">
         <v>30</v>
       </c>
@@ -3135,13 +3142,11 @@
       <c r="G123" s="20"/>
       <c r="H123" s="20"/>
       <c r="I123" s="21"/>
-      <c r="J123" s="21">
-        <v>1</v>
-      </c>
+      <c r="J123" s="21"/>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="28"/>
-      <c r="B124" s="33"/>
+      <c r="A124" s="31"/>
+      <c r="B124" s="29"/>
       <c r="C124" s="18" t="s">
         <v>22</v>
       </c>
@@ -3154,8 +3159,8 @@
       <c r="J124" s="21"/>
     </row>
     <row r="125" spans="1:10">
-      <c r="A125" s="28"/>
-      <c r="B125" s="33"/>
+      <c r="A125" s="31"/>
+      <c r="B125" s="29"/>
       <c r="C125" s="6" t="s">
         <v>71</v>
       </c>
@@ -3170,8 +3175,8 @@
       <c r="J125" s="21"/>
     </row>
     <row r="126" spans="1:10">
-      <c r="A126" s="28"/>
-      <c r="B126" s="33"/>
+      <c r="A126" s="31"/>
+      <c r="B126" s="29"/>
       <c r="C126" s="6" t="s">
         <v>70</v>
       </c>
@@ -3186,8 +3191,8 @@
       <c r="J126" s="21"/>
     </row>
     <row r="127" spans="1:10">
-      <c r="A127" s="28"/>
-      <c r="B127" s="33"/>
+      <c r="A127" s="31"/>
+      <c r="B127" s="29"/>
       <c r="C127" s="6" t="s">
         <v>72</v>
       </c>
@@ -3202,8 +3207,8 @@
       <c r="J127" s="21"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="28"/>
-      <c r="B128" s="33"/>
+      <c r="A128" s="31"/>
+      <c r="B128" s="29"/>
       <c r="C128" s="6" t="s">
         <v>73</v>
       </c>
@@ -3218,8 +3223,8 @@
       <c r="J128" s="21"/>
     </row>
     <row r="129" spans="1:10">
-      <c r="A129" s="28"/>
-      <c r="B129" s="33"/>
+      <c r="A129" s="31"/>
+      <c r="B129" s="29"/>
       <c r="C129" s="18" t="s">
         <v>23</v>
       </c>
@@ -3231,8 +3236,8 @@
       <c r="J129" s="21"/>
     </row>
     <row r="130" spans="1:10">
-      <c r="A130" s="28"/>
-      <c r="B130" s="33"/>
+      <c r="A130" s="31"/>
+      <c r="B130" s="29"/>
       <c r="C130" s="6" t="s">
         <v>71</v>
       </c>
@@ -3247,14 +3252,15 @@
       <c r="J130" s="21"/>
     </row>
     <row r="131" spans="1:10">
-      <c r="A131" s="28"/>
-      <c r="B131" s="33"/>
+      <c r="A131" s="31"/>
+      <c r="B131" s="29"/>
       <c r="C131" s="6" t="s">
         <v>70</v>
       </c>
       <c r="D131" s="20" t="s">
         <v>83</v>
       </c>
+      <c r="E131" s="20"/>
       <c r="F131" s="20"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
@@ -3262,8 +3268,8 @@
       <c r="J131" s="21"/>
     </row>
     <row r="132" spans="1:10">
-      <c r="A132" s="28"/>
-      <c r="B132" s="33"/>
+      <c r="A132" s="31"/>
+      <c r="B132" s="29"/>
       <c r="C132" s="6" t="s">
         <v>72</v>
       </c>
@@ -3278,8 +3284,8 @@
       <c r="J132" s="21"/>
     </row>
     <row r="133" spans="1:10">
-      <c r="A133" s="28"/>
-      <c r="B133" s="33"/>
+      <c r="A133" s="31"/>
+      <c r="B133" s="29"/>
       <c r="C133" s="6" t="s">
         <v>73</v>
       </c>
@@ -3294,10 +3300,10 @@
       <c r="J133" s="21"/>
     </row>
     <row r="134" spans="1:10">
-      <c r="A134" s="27">
+      <c r="A134" s="30">
         <v>6</v>
       </c>
-      <c r="B134" s="30" t="s">
+      <c r="B134" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C134" s="18" t="s">
@@ -3312,8 +3318,8 @@
       <c r="J134" s="21"/>
     </row>
     <row r="135" spans="1:10">
-      <c r="A135" s="28"/>
-      <c r="B135" s="31"/>
+      <c r="A135" s="31"/>
+      <c r="B135" s="34"/>
       <c r="C135" s="6" t="s">
         <v>98</v>
       </c>
@@ -3328,8 +3334,8 @@
       <c r="J135" s="21"/>
     </row>
     <row r="136" spans="1:10">
-      <c r="A136" s="28"/>
-      <c r="B136" s="31"/>
+      <c r="A136" s="31"/>
+      <c r="B136" s="34"/>
       <c r="C136" s="6" t="s">
         <v>67</v>
       </c>
@@ -3344,8 +3350,8 @@
       <c r="J136" s="21"/>
     </row>
     <row r="137" spans="1:10">
-      <c r="A137" s="28"/>
-      <c r="B137" s="31"/>
+      <c r="A137" s="31"/>
+      <c r="B137" s="34"/>
       <c r="C137" s="18" t="s">
         <v>74</v>
       </c>
@@ -3358,8 +3364,8 @@
       <c r="J137" s="21"/>
     </row>
     <row r="138" spans="1:10">
-      <c r="A138" s="28"/>
-      <c r="B138" s="31"/>
+      <c r="A138" s="31"/>
+      <c r="B138" s="34"/>
       <c r="C138" s="6" t="s">
         <v>69</v>
       </c>
@@ -3374,8 +3380,8 @@
       <c r="J138" s="21"/>
     </row>
     <row r="139" spans="1:10">
-      <c r="A139" s="28"/>
-      <c r="B139" s="31"/>
+      <c r="A139" s="31"/>
+      <c r="B139" s="34"/>
       <c r="C139" s="6" t="s">
         <v>59</v>
       </c>
@@ -3390,8 +3396,8 @@
       <c r="J139" s="21"/>
     </row>
     <row r="140" spans="1:10">
-      <c r="A140" s="28"/>
-      <c r="B140" s="31"/>
+      <c r="A140" s="31"/>
+      <c r="B140" s="34"/>
       <c r="C140" s="18" t="s">
         <v>75</v>
       </c>
@@ -3404,8 +3410,8 @@
       <c r="J140" s="21"/>
     </row>
     <row r="141" spans="1:10">
-      <c r="A141" s="28"/>
-      <c r="B141" s="31"/>
+      <c r="A141" s="31"/>
+      <c r="B141" s="34"/>
       <c r="C141" s="6" t="s">
         <v>70</v>
       </c>
@@ -3420,8 +3426,8 @@
       <c r="J141" s="21"/>
     </row>
     <row r="142" spans="1:10">
-      <c r="A142" s="28"/>
-      <c r="B142" s="31"/>
+      <c r="A142" s="31"/>
+      <c r="B142" s="34"/>
       <c r="C142" s="6" t="s">
         <v>76</v>
       </c>
@@ -3436,8 +3442,8 @@
       <c r="J142" s="21"/>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143" s="28"/>
-      <c r="B143" s="31"/>
+      <c r="A143" s="31"/>
+      <c r="B143" s="34"/>
       <c r="C143" s="25" t="s">
         <v>88</v>
       </c>
@@ -3452,8 +3458,8 @@
       <c r="J143" s="21"/>
     </row>
     <row r="144" spans="1:10">
-      <c r="A144" s="28"/>
-      <c r="B144" s="31"/>
+      <c r="A144" s="31"/>
+      <c r="B144" s="34"/>
       <c r="C144" s="18" t="s">
         <v>96</v>
       </c>
@@ -3466,8 +3472,8 @@
       <c r="J144" s="21"/>
     </row>
     <row r="145" spans="1:10">
-      <c r="A145" s="28"/>
-      <c r="B145" s="31"/>
+      <c r="A145" s="31"/>
+      <c r="B145" s="34"/>
       <c r="C145" s="6" t="s">
         <v>58</v>
       </c>
@@ -3482,8 +3488,8 @@
       <c r="J145" s="21"/>
     </row>
     <row r="146" spans="1:10">
-      <c r="A146" s="28"/>
-      <c r="B146" s="31"/>
+      <c r="A146" s="31"/>
+      <c r="B146" s="34"/>
       <c r="C146" s="6" t="s">
         <v>56</v>
       </c>
@@ -3498,8 +3504,8 @@
       <c r="J146" s="21"/>
     </row>
     <row r="147" spans="1:10">
-      <c r="A147" s="28"/>
-      <c r="B147" s="31"/>
+      <c r="A147" s="31"/>
+      <c r="B147" s="34"/>
       <c r="C147" s="6" t="s">
         <v>72</v>
       </c>
@@ -3514,8 +3520,8 @@
       <c r="J147" s="21"/>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148" s="28"/>
-      <c r="B148" s="31"/>
+      <c r="A148" s="31"/>
+      <c r="B148" s="34"/>
       <c r="C148" s="6" t="s">
         <v>73</v>
       </c>
@@ -3530,8 +3536,8 @@
       <c r="J148" s="21"/>
     </row>
     <row r="149" spans="1:10">
-      <c r="A149" s="28"/>
-      <c r="B149" s="31"/>
+      <c r="A149" s="31"/>
+      <c r="B149" s="34"/>
       <c r="C149" s="6" t="s">
         <v>62</v>
       </c>
@@ -3546,8 +3552,8 @@
       <c r="J149" s="21"/>
     </row>
     <row r="150" spans="1:10">
-      <c r="A150" s="28"/>
-      <c r="B150" s="31"/>
+      <c r="A150" s="31"/>
+      <c r="B150" s="34"/>
       <c r="C150" s="26" t="s">
         <v>77</v>
       </c>
@@ -3562,8 +3568,8 @@
       <c r="J150" s="21"/>
     </row>
     <row r="151" spans="1:10">
-      <c r="A151" s="28"/>
-      <c r="B151" s="31"/>
+      <c r="A151" s="31"/>
+      <c r="B151" s="34"/>
       <c r="C151" s="18" t="s">
         <v>97</v>
       </c>
@@ -3576,8 +3582,8 @@
       <c r="J151" s="21"/>
     </row>
     <row r="152" spans="1:10">
-      <c r="A152" s="28"/>
-      <c r="B152" s="31"/>
+      <c r="A152" s="31"/>
+      <c r="B152" s="34"/>
       <c r="C152" s="6" t="s">
         <v>72</v>
       </c>
@@ -3592,8 +3598,8 @@
       <c r="J152" s="21"/>
     </row>
     <row r="153" spans="1:10">
-      <c r="A153" s="28"/>
-      <c r="B153" s="31"/>
+      <c r="A153" s="31"/>
+      <c r="B153" s="34"/>
       <c r="C153" s="6" t="s">
         <v>73</v>
       </c>
@@ -3608,8 +3614,8 @@
       <c r="J153" s="21"/>
     </row>
     <row r="154" spans="1:10">
-      <c r="A154" s="28"/>
-      <c r="B154" s="31"/>
+      <c r="A154" s="31"/>
+      <c r="B154" s="34"/>
       <c r="C154" s="6" t="s">
         <v>62</v>
       </c>
@@ -3624,8 +3630,8 @@
       <c r="J154" s="21"/>
     </row>
     <row r="155" spans="1:10">
-      <c r="A155" s="28"/>
-      <c r="B155" s="31"/>
+      <c r="A155" s="31"/>
+      <c r="B155" s="34"/>
       <c r="C155" s="26" t="s">
         <v>77</v>
       </c>
@@ -3640,8 +3646,8 @@
       <c r="J155" s="21"/>
     </row>
     <row r="156" spans="1:10">
-      <c r="A156" s="29"/>
-      <c r="B156" s="32"/>
+      <c r="A156" s="32"/>
+      <c r="B156" s="28"/>
       <c r="C156" s="18"/>
       <c r="D156" s="20"/>
       <c r="E156" s="20"/>
@@ -3892,18 +3898,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A134:A156"/>
+    <mergeCell ref="B134:B156"/>
+    <mergeCell ref="B54:B133"/>
+    <mergeCell ref="A54:A133"/>
+    <mergeCell ref="B29:B53"/>
+    <mergeCell ref="A29:A53"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B12:B28"/>
     <mergeCell ref="A12:A28"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A134:A156"/>
-    <mergeCell ref="B134:B156"/>
-    <mergeCell ref="B54:B133"/>
-    <mergeCell ref="A54:A133"/>
-    <mergeCell ref="B29:B53"/>
-    <mergeCell ref="A29:A53"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D18 D2:H15 F16:H18 D22 D19:H21 F22:H22 D26 F26:H26 D23:H25 D92:D128 D130:D177 F92:H177 E132:E177 D27:H91 E93:E130">

</xml_diff>

<commit_message>
Update final report, short report, slide, tasksheet
</commit_message>
<xml_diff>
--- a/Other/Tmp/Tasksheet Final.xlsx
+++ b/Other/Tmp/Tasksheet Final.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="142">
   <si>
     <t>No.</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Traffic Detect</t>
   </si>
   <si>
-    <t>Traffice Recognize</t>
-  </si>
-  <si>
     <t>Mobile Client</t>
   </si>
   <si>
@@ -531,13 +528,40 @@
   </si>
   <si>
     <t>View</t>
+  </si>
+  <si>
+    <t>Traffic Recognize</t>
+  </si>
+  <si>
+    <t>Fix wrong information</t>
+  </si>
+  <si>
+    <t>Fix wrong recognition</t>
+  </si>
+  <si>
+    <t>Configure system</t>
+  </si>
+  <si>
+    <t>Add traffic sign</t>
+  </si>
+  <si>
+    <t>View report</t>
+  </si>
+  <si>
+    <t>Add favorite</t>
+  </si>
+  <si>
+    <t>Search traffic sign</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +623,11 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -695,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -782,6 +811,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="8"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1088,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J179"/>
+  <dimension ref="A1:J193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1115,16 +1150,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="H1" s="13"/>
       <c r="I1" s="8" t="s">
@@ -1145,7 +1180,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1161,7 +1196,7 @@
         <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1174,10 +1209,10 @@
       <c r="A4" s="29"/>
       <c r="B4" s="29"/>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1193,7 +1228,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1209,7 +1244,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1225,7 +1260,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1245,7 +1280,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1261,7 +1296,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1277,7 +1312,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1293,7 +1328,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1314,7 +1349,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -1344,7 +1379,7 @@
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -1369,12 +1404,10 @@
     <row r="16" spans="1:10">
       <c r="A16" s="29"/>
       <c r="B16" s="29"/>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -1385,11 +1418,11 @@
     <row r="17" spans="1:10">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
-      <c r="C17" s="19" t="s">
-        <v>45</v>
+      <c r="C17" s="36" t="s">
+        <v>68</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
@@ -1401,11 +1434,11 @@
     <row r="18" spans="1:10">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
-      <c r="C18" s="19" t="s">
-        <v>46</v>
+      <c r="C18" s="36" t="s">
+        <v>136</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
@@ -1417,13 +1450,11 @@
     <row r="19" spans="1:10">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
-      <c r="C19" s="19" t="s">
-        <v>57</v>
+      <c r="C19" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="D19" s="20"/>
-      <c r="E19" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -1433,13 +1464,13 @@
     <row r="20" spans="1:10">
       <c r="A20" s="29"/>
       <c r="B20" s="29"/>
-      <c r="C20" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C20" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -1449,11 +1480,13 @@
     <row r="21" spans="1:10">
       <c r="A21" s="29"/>
       <c r="B21" s="29"/>
-      <c r="C21" s="23" t="s">
-        <v>16</v>
+      <c r="C21" s="36" t="s">
+        <v>138</v>
       </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
+      <c r="E21" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -1463,11 +1496,11 @@
     <row r="22" spans="1:10">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
-      <c r="C22" s="19" t="s">
-        <v>17</v>
+      <c r="C22" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
@@ -1479,13 +1512,11 @@
     <row r="23" spans="1:10">
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
-      <c r="C23" s="19" t="s">
-        <v>18</v>
+      <c r="C23" s="35" t="s">
+        <v>57</v>
       </c>
       <c r="D23" s="20"/>
-      <c r="E23" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -1495,12 +1526,12 @@
     <row r="24" spans="1:10">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
-      <c r="C24" s="19" t="s">
-        <v>48</v>
+      <c r="C24" s="36" t="s">
+        <v>139</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -1511,12 +1542,12 @@
     <row r="25" spans="1:10">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
-      <c r="C25" s="19" t="s">
-        <v>102</v>
+      <c r="C25" s="36" t="s">
+        <v>109</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -1527,12 +1558,10 @@
     <row r="26" spans="1:10">
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
-      <c r="C26" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C26" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -1543,11 +1572,11 @@
     <row r="27" spans="1:10">
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
-      <c r="C27" s="7" t="s">
-        <v>50</v>
+      <c r="C27" s="36" t="s">
+        <v>140</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
@@ -1559,12 +1588,10 @@
     <row r="28" spans="1:10">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
-      <c r="C28" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C28" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -1573,16 +1600,12 @@
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
@@ -1591,13 +1614,13 @@
       <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="4" t="s">
-        <v>52</v>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -1607,15 +1630,15 @@
       <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="20"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -1623,15 +1646,15 @@
       <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="20"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -1639,13 +1662,15 @@
       <c r="J32" s="21"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="5" t="s">
-        <v>103</v>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+      <c r="E33" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
@@ -1653,15 +1678,15 @@
       <c r="J33" s="21"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -1669,15 +1694,15 @@
       <c r="J34" s="21"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="20"/>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
@@ -1685,15 +1710,15 @@
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="20"/>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
@@ -1701,15 +1726,17 @@
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="20"/>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
@@ -1719,13 +1746,13 @@
     <row r="38" spans="1:10">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-      <c r="C38" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="20"/>
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
@@ -1735,13 +1762,13 @@
     <row r="39" spans="1:10">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="20"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -1751,13 +1778,13 @@
     <row r="40" spans="1:10">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="20"/>
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
@@ -1767,8 +1794,8 @@
     <row r="41" spans="1:10">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
-      <c r="C41" s="18" t="s">
-        <v>21</v>
+      <c r="C41" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
@@ -1782,12 +1809,12 @@
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
       <c r="C42" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" s="20"/>
+        <v>104</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F42" s="20"/>
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
@@ -1798,12 +1825,12 @@
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
       <c r="C43" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E43" s="20"/>
+        <v>103</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
@@ -1814,12 +1841,12 @@
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
       <c r="C44" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="20"/>
+        <v>105</v>
+      </c>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
@@ -1830,11 +1857,11 @@
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
       <c r="C45" s="19" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F45" s="20"/>
       <c r="G45" s="20"/>
@@ -1845,12 +1872,12 @@
     <row r="46" spans="1:10">
       <c r="A46" s="34"/>
       <c r="B46" s="34"/>
-      <c r="C46" s="24" t="s">
-        <v>87</v>
+      <c r="C46" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="20"/>
@@ -1861,11 +1888,13 @@
     <row r="47" spans="1:10">
       <c r="A47" s="34"/>
       <c r="B47" s="34"/>
-      <c r="C47" s="5" t="s">
-        <v>54</v>
+      <c r="C47" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
+      <c r="E47" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F47" s="20"/>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
@@ -1876,12 +1905,12 @@
       <c r="A48" s="34"/>
       <c r="B48" s="34"/>
       <c r="C48" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" s="20"/>
+        <v>109</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F48" s="20"/>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
@@ -1891,12 +1920,10 @@
     <row r="49" spans="1:10">
       <c r="A49" s="34"/>
       <c r="B49" s="34"/>
-      <c r="C49" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C49" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
@@ -1907,10 +1934,12 @@
     <row r="50" spans="1:10">
       <c r="A50" s="34"/>
       <c r="B50" s="34"/>
-      <c r="C50" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50" s="20"/>
+      <c r="C50" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
@@ -1922,10 +1951,10 @@
       <c r="A51" s="34"/>
       <c r="B51" s="34"/>
       <c r="C51" s="19" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
@@ -1938,10 +1967,10 @@
       <c r="A52" s="34"/>
       <c r="B52" s="34"/>
       <c r="C52" s="19" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
@@ -1951,14 +1980,14 @@
       <c r="J52" s="21"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="24" t="s">
-        <v>111</v>
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
@@ -1967,17 +1996,15 @@
       <c r="J53" s="21"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="30">
-        <v>5</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>24</v>
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
+      <c r="E54" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
@@ -1985,14 +2012,12 @@
       <c r="J54" s="21"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="31"/>
-      <c r="B55" s="29"/>
-      <c r="C55" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A55" s="34"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
       <c r="G55" s="20"/>
@@ -2001,15 +2026,15 @@
       <c r="J55" s="21"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="31"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A56" s="34"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="20"/>
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
@@ -2017,12 +2042,14 @@
       <c r="J56" s="21"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="31"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" s="20"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E57" s="20"/>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -2031,48 +2058,44 @@
       <c r="J57" s="21"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="31"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="20"/>
       <c r="E58" s="20"/>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
       <c r="I58" s="21"/>
-      <c r="J58" s="21">
-        <v>4</v>
-      </c>
+      <c r="J58" s="21"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="31"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="6" t="s">
-        <v>66</v>
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="20"/>
       <c r="G59" s="20"/>
       <c r="H59" s="20"/>
       <c r="I59" s="21"/>
-      <c r="J59" s="21">
-        <v>4</v>
-      </c>
+      <c r="J59" s="21"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="31"/>
-      <c r="B60" s="29"/>
-      <c r="C60" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="20"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
       <c r="G60" s="20"/>
@@ -2081,82 +2104,76 @@
       <c r="J60" s="21"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="31"/>
-      <c r="B61" s="29"/>
-      <c r="C61" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E61" s="20"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F61" s="20"/>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
       <c r="I61" s="21"/>
-      <c r="J61" s="21">
-        <v>1</v>
-      </c>
+      <c r="J61" s="21"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="31"/>
-      <c r="B62" s="29"/>
-      <c r="C62" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A62" s="30">
+        <v>5</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="20"/>
       <c r="E62" s="20"/>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
       <c r="I62" s="21"/>
-      <c r="J62" s="21">
-        <v>1</v>
-      </c>
+      <c r="J62" s="21"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="31"/>
       <c r="B63" s="29"/>
       <c r="C63" s="6" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
       <c r="I63" s="21"/>
-      <c r="J63" s="21">
-        <v>1</v>
-      </c>
+      <c r="J63" s="21"/>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="31"/>
       <c r="B64" s="29"/>
       <c r="C64" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E64" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F64" s="20"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
       <c r="I64" s="21"/>
-      <c r="J64" s="21">
-        <v>1</v>
-      </c>
+      <c r="J64" s="21"/>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="31"/>
       <c r="B65" s="29"/>
-      <c r="C65" s="27" t="s">
-        <v>69</v>
+      <c r="C65" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
@@ -2169,11 +2186,11 @@
     <row r="66" spans="1:10">
       <c r="A66" s="31"/>
       <c r="B66" s="29"/>
-      <c r="C66" s="19" t="s">
-        <v>112</v>
+      <c r="C66" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
@@ -2181,17 +2198,17 @@
       <c r="H66" s="20"/>
       <c r="I66" s="21"/>
       <c r="J66" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="31"/>
       <c r="B67" s="29"/>
-      <c r="C67" s="19" t="s">
-        <v>113</v>
+      <c r="C67" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
@@ -2199,14 +2216,14 @@
       <c r="H67" s="20"/>
       <c r="I67" s="21"/>
       <c r="J67" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="31"/>
       <c r="B68" s="29"/>
-      <c r="C68" s="27" t="s">
-        <v>70</v>
+      <c r="C68" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="D68" s="20"/>
       <c r="E68" s="20"/>
@@ -2219,11 +2236,11 @@
     <row r="69" spans="1:10">
       <c r="A69" s="31"/>
       <c r="B69" s="29"/>
-      <c r="C69" s="19" t="s">
-        <v>114</v>
+      <c r="C69" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="20"/>
@@ -2238,10 +2255,10 @@
       <c r="A70" s="31"/>
       <c r="B70" s="29"/>
       <c r="C70" s="6" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
@@ -2255,25 +2272,29 @@
     <row r="71" spans="1:10">
       <c r="A71" s="31"/>
       <c r="B71" s="29"/>
-      <c r="C71" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D71" s="20"/>
+      <c r="C71" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
       <c r="G71" s="20"/>
       <c r="H71" s="20"/>
       <c r="I71" s="21"/>
-      <c r="J71" s="21"/>
+      <c r="J71" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="31"/>
       <c r="B72" s="29"/>
-      <c r="C72" s="19" t="s">
-        <v>115</v>
+      <c r="C72" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="20"/>
@@ -2287,43 +2308,43 @@
     <row r="73" spans="1:10">
       <c r="A73" s="31"/>
       <c r="B73" s="29"/>
-      <c r="C73" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C73" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" s="20"/>
       <c r="E73" s="20"/>
       <c r="F73" s="20"/>
       <c r="G73" s="20"/>
       <c r="H73" s="20"/>
       <c r="I73" s="21"/>
-      <c r="J73" s="21">
-        <v>1</v>
-      </c>
+      <c r="J73" s="21"/>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="31"/>
       <c r="B74" s="29"/>
-      <c r="C74" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D74" s="20"/>
+      <c r="C74" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E74" s="20"/>
       <c r="F74" s="20"/>
       <c r="G74" s="20"/>
       <c r="H74" s="20"/>
       <c r="I74" s="21"/>
-      <c r="J74" s="21"/>
+      <c r="J74" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="31"/>
       <c r="B75" s="29"/>
       <c r="C75" s="19" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E75" s="20"/>
       <c r="F75" s="20"/>
@@ -2337,29 +2358,25 @@
     <row r="76" spans="1:10">
       <c r="A76" s="31"/>
       <c r="B76" s="29"/>
-      <c r="C76" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C76" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" s="20"/>
       <c r="E76" s="20"/>
       <c r="F76" s="20"/>
       <c r="G76" s="20"/>
       <c r="H76" s="20"/>
       <c r="I76" s="21"/>
-      <c r="J76" s="21">
-        <v>2</v>
-      </c>
+      <c r="J76" s="21"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="31"/>
       <c r="B77" s="29"/>
-      <c r="C77" s="6" t="s">
-        <v>101</v>
+      <c r="C77" s="19" t="s">
+        <v>113</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="20"/>
@@ -2367,14 +2384,14 @@
       <c r="H77" s="20"/>
       <c r="I77" s="21"/>
       <c r="J77" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="31"/>
       <c r="B78" s="29"/>
-      <c r="C78" s="5" t="s">
-        <v>68</v>
+      <c r="C78" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="D78" s="20"/>
       <c r="E78" s="20"/>
@@ -2387,11 +2404,11 @@
     <row r="79" spans="1:10">
       <c r="A79" s="31"/>
       <c r="B79" s="29"/>
-      <c r="C79" s="6" t="s">
-        <v>58</v>
+      <c r="C79" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="20"/>
@@ -2405,11 +2422,11 @@
     <row r="80" spans="1:10">
       <c r="A80" s="31"/>
       <c r="B80" s="29"/>
-      <c r="C80" s="6" t="s">
-        <v>100</v>
+      <c r="C80" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="20"/>
@@ -2423,43 +2440,43 @@
     <row r="81" spans="1:10">
       <c r="A81" s="31"/>
       <c r="B81" s="29"/>
-      <c r="C81" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D81" s="20"/>
+      <c r="C81" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E81" s="20"/>
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
       <c r="I81" s="21"/>
-      <c r="J81" s="21"/>
+      <c r="J81" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="31"/>
       <c r="B82" s="29"/>
-      <c r="C82" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D82" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C82" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D82" s="20"/>
       <c r="E82" s="20"/>
       <c r="F82" s="20"/>
       <c r="G82" s="20"/>
       <c r="H82" s="20"/>
       <c r="I82" s="21"/>
-      <c r="J82" s="21">
-        <v>1</v>
-      </c>
+      <c r="J82" s="21"/>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="31"/>
       <c r="B83" s="29"/>
       <c r="C83" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="20"/>
@@ -2473,43 +2490,43 @@
     <row r="84" spans="1:10">
       <c r="A84" s="31"/>
       <c r="B84" s="29"/>
-      <c r="C84" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="D84" s="20"/>
+      <c r="C84" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E84" s="20"/>
       <c r="F84" s="20"/>
       <c r="G84" s="20"/>
       <c r="H84" s="20"/>
       <c r="I84" s="21"/>
-      <c r="J84" s="21"/>
+      <c r="J84" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="31"/>
       <c r="B85" s="29"/>
-      <c r="C85" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D85" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C85" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" s="20"/>
       <c r="E85" s="20"/>
       <c r="F85" s="20"/>
       <c r="G85" s="20"/>
       <c r="H85" s="20"/>
       <c r="I85" s="21"/>
-      <c r="J85" s="21">
-        <v>2</v>
-      </c>
+      <c r="J85" s="21"/>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="31"/>
       <c r="B86" s="29"/>
-      <c r="C86" s="6" t="s">
-        <v>91</v>
+      <c r="C86" s="19" t="s">
+        <v>117</v>
       </c>
       <c r="D86" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="20"/>
@@ -2523,25 +2540,29 @@
     <row r="87" spans="1:10">
       <c r="A87" s="31"/>
       <c r="B87" s="29"/>
-      <c r="C87" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D87" s="20"/>
+      <c r="C87" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E87" s="20"/>
       <c r="F87" s="20"/>
       <c r="G87" s="20"/>
       <c r="H87" s="20"/>
       <c r="I87" s="21"/>
-      <c r="J87" s="21"/>
+      <c r="J87" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="31"/>
       <c r="B88" s="29"/>
-      <c r="C88" s="19" t="s">
-        <v>115</v>
+      <c r="C88" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="20"/>
@@ -2549,35 +2570,31 @@
       <c r="H88" s="20"/>
       <c r="I88" s="21"/>
       <c r="J88" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="31"/>
       <c r="B89" s="29"/>
-      <c r="C89" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="D89" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C89" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D89" s="20"/>
       <c r="E89" s="20"/>
       <c r="F89" s="20"/>
       <c r="G89" s="20"/>
       <c r="H89" s="20"/>
       <c r="I89" s="21"/>
-      <c r="J89" s="21">
-        <v>1</v>
-      </c>
+      <c r="J89" s="21"/>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="31"/>
       <c r="B90" s="29"/>
       <c r="C90" s="6" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="20"/>
@@ -2592,12 +2609,12 @@
       <c r="A91" s="31"/>
       <c r="B91" s="29"/>
       <c r="C91" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D91" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E91" s="20"/>
       <c r="F91" s="20"/>
       <c r="G91" s="20"/>
       <c r="H91" s="20"/>
@@ -2609,45 +2626,45 @@
     <row r="92" spans="1:10">
       <c r="A92" s="31"/>
       <c r="B92" s="29"/>
-      <c r="C92" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C92" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D92" s="20"/>
       <c r="E92" s="20"/>
       <c r="F92" s="20"/>
       <c r="G92" s="20"/>
       <c r="H92" s="20"/>
       <c r="I92" s="21"/>
-      <c r="J92" s="21">
-        <v>2</v>
-      </c>
+      <c r="J92" s="21"/>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="31"/>
       <c r="B93" s="29"/>
-      <c r="C93" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D93" s="20"/>
+      <c r="C93" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D93" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E93" s="20"/>
       <c r="F93" s="20"/>
       <c r="G93" s="20"/>
       <c r="H93" s="20"/>
       <c r="I93" s="21"/>
-      <c r="J93" s="21"/>
+      <c r="J93" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="31"/>
       <c r="B94" s="29"/>
       <c r="C94" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E94" s="20"/>
       <c r="F94" s="20"/>
       <c r="G94" s="20"/>
       <c r="H94" s="20"/>
@@ -2659,42 +2676,40 @@
     <row r="95" spans="1:10">
       <c r="A95" s="31"/>
       <c r="B95" s="29"/>
-      <c r="C95" s="19" t="s">
-        <v>133</v>
+      <c r="C95" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="D95" s="20"/>
-      <c r="E95" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E95" s="20"/>
       <c r="F95" s="20"/>
       <c r="G95" s="20"/>
       <c r="H95" s="20"/>
       <c r="I95" s="21"/>
-      <c r="J95" s="21">
-        <v>1</v>
-      </c>
+      <c r="J95" s="21"/>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="31"/>
       <c r="B96" s="29"/>
-      <c r="C96" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C96" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E96" s="20"/>
       <c r="F96" s="20"/>
       <c r="G96" s="20"/>
       <c r="H96" s="20"/>
       <c r="I96" s="21"/>
-      <c r="J96" s="21"/>
+      <c r="J96" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="31"/>
       <c r="B97" s="29"/>
-      <c r="C97" s="19" t="s">
-        <v>120</v>
+      <c r="C97" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="D97" s="20"/>
       <c r="E97" s="20"/>
@@ -2702,52 +2717,54 @@
       <c r="G97" s="20"/>
       <c r="H97" s="20"/>
       <c r="I97" s="21"/>
-      <c r="J97" s="21">
-        <v>1</v>
-      </c>
+      <c r="J97" s="21"/>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="31"/>
       <c r="B98" s="29"/>
-      <c r="C98" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D98" s="20"/>
+      <c r="C98" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D98" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E98" s="20"/>
       <c r="F98" s="20"/>
       <c r="G98" s="20"/>
       <c r="H98" s="20"/>
       <c r="I98" s="21"/>
-      <c r="J98" s="21"/>
+      <c r="J98" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="31"/>
       <c r="B99" s="29"/>
       <c r="C99" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D99" s="20"/>
-      <c r="E99" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E99" s="20"/>
       <c r="F99" s="20"/>
       <c r="G99" s="20"/>
       <c r="H99" s="20"/>
       <c r="I99" s="21"/>
       <c r="J99" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="31"/>
       <c r="B100" s="29"/>
-      <c r="C100" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D100" s="20"/>
-      <c r="E100" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C100" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D100" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E100" s="20"/>
       <c r="F100" s="20"/>
       <c r="G100" s="20"/>
       <c r="H100" s="20"/>
@@ -2759,8 +2776,8 @@
     <row r="101" spans="1:10">
       <c r="A101" s="31"/>
       <c r="B101" s="29"/>
-      <c r="C101" s="5" t="s">
-        <v>67</v>
+      <c r="C101" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="D101" s="20"/>
       <c r="E101" s="20"/>
@@ -2773,13 +2790,13 @@
     <row r="102" spans="1:10">
       <c r="A102" s="31"/>
       <c r="B102" s="29"/>
-      <c r="C102" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D102" s="20"/>
-      <c r="E102" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C102" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E102" s="20"/>
       <c r="F102" s="20"/>
       <c r="G102" s="20"/>
       <c r="H102" s="20"/>
@@ -2791,13 +2808,13 @@
     <row r="103" spans="1:10">
       <c r="A103" s="31"/>
       <c r="B103" s="29"/>
-      <c r="C103" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D103" s="20"/>
-      <c r="E103" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C103" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E103" s="20"/>
       <c r="F103" s="20"/>
       <c r="G103" s="20"/>
       <c r="H103" s="20"/>
@@ -2809,26 +2826,30 @@
     <row r="104" spans="1:10">
       <c r="A104" s="31"/>
       <c r="B104" s="29"/>
-      <c r="C104" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D104" s="20"/>
+      <c r="C104" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D104" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E104" s="20"/>
       <c r="F104" s="20"/>
       <c r="G104" s="20"/>
       <c r="H104" s="20"/>
       <c r="I104" s="21"/>
-      <c r="J104" s="21"/>
+      <c r="J104" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="31"/>
       <c r="B105" s="29"/>
-      <c r="C105" s="19" t="s">
-        <v>123</v>
+      <c r="C105" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D105" s="20"/>
       <c r="E105" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F105" s="20"/>
       <c r="G105" s="20"/>
@@ -2841,26 +2862,26 @@
     <row r="106" spans="1:10">
       <c r="A106" s="31"/>
       <c r="B106" s="29"/>
-      <c r="C106" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D106" s="20"/>
-      <c r="E106" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C106" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D106" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E106" s="20"/>
       <c r="F106" s="20"/>
       <c r="G106" s="20"/>
       <c r="H106" s="20"/>
       <c r="I106" s="21"/>
       <c r="J106" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="31"/>
       <c r="B107" s="29"/>
       <c r="C107" s="27" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D107" s="20"/>
       <c r="E107" s="20"/>
@@ -2874,11 +2895,11 @@
       <c r="A108" s="31"/>
       <c r="B108" s="29"/>
       <c r="C108" s="19" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D108" s="20"/>
       <c r="E108" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F108" s="20"/>
       <c r="G108" s="20"/>
@@ -2892,11 +2913,11 @@
       <c r="A109" s="31"/>
       <c r="B109" s="29"/>
       <c r="C109" s="19" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D109" s="20"/>
       <c r="E109" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F109" s="20"/>
       <c r="G109" s="20"/>
@@ -2909,80 +2930,76 @@
     <row r="110" spans="1:10">
       <c r="A110" s="31"/>
       <c r="B110" s="29"/>
-      <c r="C110" s="19" t="s">
-        <v>127</v>
+      <c r="C110" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="D110" s="20"/>
       <c r="E110" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F110" s="20"/>
       <c r="G110" s="20"/>
       <c r="H110" s="20"/>
       <c r="I110" s="21"/>
-      <c r="J110" s="21">
-        <v>3</v>
-      </c>
+      <c r="J110" s="21"/>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="31"/>
       <c r="B111" s="29"/>
       <c r="C111" s="19" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D111" s="20"/>
-      <c r="E111" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E111" s="20"/>
       <c r="F111" s="20"/>
       <c r="G111" s="20"/>
       <c r="H111" s="20"/>
       <c r="I111" s="21"/>
       <c r="J111" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="31"/>
       <c r="B112" s="29"/>
-      <c r="C112" s="19" t="s">
-        <v>129</v>
+      <c r="C112" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="D112" s="20"/>
-      <c r="E112" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E112" s="20"/>
       <c r="F112" s="20"/>
       <c r="G112" s="20"/>
       <c r="H112" s="20"/>
       <c r="I112" s="21"/>
-      <c r="J112" s="21">
-        <v>2</v>
-      </c>
+      <c r="J112" s="21"/>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="31"/>
       <c r="B113" s="29"/>
-      <c r="C113" s="27" t="s">
-        <v>94</v>
+      <c r="C113" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
+      <c r="E113" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F113" s="20"/>
       <c r="G113" s="20"/>
       <c r="H113" s="20"/>
       <c r="I113" s="21"/>
-      <c r="J113" s="21"/>
+      <c r="J113" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="31"/>
       <c r="B114" s="29"/>
       <c r="C114" s="19" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D114" s="20"/>
       <c r="E114" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F114" s="20"/>
       <c r="G114" s="20"/>
@@ -2995,44 +3012,44 @@
     <row r="115" spans="1:10">
       <c r="A115" s="31"/>
       <c r="B115" s="29"/>
-      <c r="C115" s="19" t="s">
-        <v>111</v>
+      <c r="C115" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="D115" s="20"/>
-      <c r="E115" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E115" s="20"/>
       <c r="F115" s="20"/>
       <c r="G115" s="20"/>
       <c r="H115" s="20"/>
       <c r="I115" s="21"/>
-      <c r="J115" s="21">
-        <v>3</v>
-      </c>
+      <c r="J115" s="21"/>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="31"/>
       <c r="B116" s="29"/>
-      <c r="C116" s="27" t="s">
-        <v>95</v>
+      <c r="C116" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="D116" s="20"/>
-      <c r="E116" s="20"/>
+      <c r="E116" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F116" s="20"/>
       <c r="G116" s="20"/>
       <c r="H116" s="20"/>
       <c r="I116" s="21"/>
-      <c r="J116" s="21"/>
+      <c r="J116" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="31"/>
       <c r="B117" s="29"/>
-      <c r="C117" s="19" t="s">
-        <v>120</v>
+      <c r="C117" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D117" s="20"/>
       <c r="E117" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F117" s="20"/>
       <c r="G117" s="20"/>
@@ -3045,44 +3062,44 @@
     <row r="118" spans="1:10">
       <c r="A118" s="31"/>
       <c r="B118" s="29"/>
-      <c r="C118" s="6" t="s">
-        <v>131</v>
+      <c r="C118" s="27" t="s">
+        <v>86</v>
       </c>
       <c r="D118" s="20"/>
-      <c r="E118" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E118" s="20"/>
       <c r="F118" s="20"/>
       <c r="G118" s="20"/>
       <c r="H118" s="20"/>
       <c r="I118" s="21"/>
-      <c r="J118" s="21">
-        <v>2</v>
-      </c>
+      <c r="J118" s="21"/>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="31"/>
       <c r="B119" s="29"/>
-      <c r="C119" s="27" t="s">
-        <v>99</v>
+      <c r="C119" s="19" t="s">
+        <v>122</v>
       </c>
       <c r="D119" s="20"/>
-      <c r="E119" s="20"/>
+      <c r="E119" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F119" s="20"/>
       <c r="G119" s="20"/>
       <c r="H119" s="20"/>
       <c r="I119" s="21"/>
-      <c r="J119" s="21"/>
+      <c r="J119" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="31"/>
       <c r="B120" s="29"/>
       <c r="C120" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D120" s="20"/>
       <c r="E120" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F120" s="20"/>
       <c r="G120" s="20"/>
@@ -3095,30 +3112,26 @@
     <row r="121" spans="1:10">
       <c r="A121" s="31"/>
       <c r="B121" s="29"/>
-      <c r="C121" s="19" t="s">
-        <v>122</v>
+      <c r="C121" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="D121" s="20"/>
-      <c r="E121" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E121" s="20"/>
       <c r="F121" s="20"/>
       <c r="G121" s="20"/>
       <c r="H121" s="20"/>
       <c r="I121" s="21"/>
-      <c r="J121" s="21">
-        <v>1</v>
-      </c>
+      <c r="J121" s="21"/>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="31"/>
       <c r="B122" s="29"/>
-      <c r="C122" s="6" t="s">
-        <v>132</v>
+      <c r="C122" s="19" t="s">
+        <v>124</v>
       </c>
       <c r="D122" s="20"/>
       <c r="E122" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F122" s="20"/>
       <c r="G122" s="20"/>
@@ -3131,75 +3144,83 @@
     <row r="123" spans="1:10">
       <c r="A123" s="31"/>
       <c r="B123" s="29"/>
-      <c r="C123" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D123" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E123" s="20"/>
+      <c r="C123" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D123" s="20"/>
+      <c r="E123" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F123" s="20"/>
       <c r="G123" s="20"/>
       <c r="H123" s="20"/>
       <c r="I123" s="21"/>
-      <c r="J123" s="21"/>
+      <c r="J123" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="31"/>
       <c r="B124" s="29"/>
-      <c r="C124" s="18" t="s">
-        <v>22</v>
+      <c r="C124" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="D124" s="20"/>
-      <c r="E124" s="20"/>
+      <c r="E124" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F124" s="20"/>
       <c r="G124" s="20"/>
       <c r="H124" s="20"/>
       <c r="I124" s="21"/>
-      <c r="J124" s="21"/>
+      <c r="J124" s="21">
+        <v>3</v>
+      </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="31"/>
       <c r="B125" s="29"/>
-      <c r="C125" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D125" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E125" s="20"/>
+      <c r="C125" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D125" s="20"/>
+      <c r="E125" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F125" s="20"/>
       <c r="G125" s="20"/>
       <c r="H125" s="20"/>
       <c r="I125" s="21"/>
-      <c r="J125" s="21"/>
+      <c r="J125" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="31"/>
       <c r="B126" s="29"/>
-      <c r="C126" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D126" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E126" s="20"/>
+      <c r="C126" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D126" s="20"/>
+      <c r="E126" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F126" s="20"/>
       <c r="G126" s="20"/>
       <c r="H126" s="20"/>
       <c r="I126" s="21"/>
-      <c r="J126" s="21"/>
+      <c r="J126" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="31"/>
       <c r="B127" s="29"/>
-      <c r="C127" s="6" t="s">
-        <v>72</v>
+      <c r="C127" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="D127" s="20"/>
-      <c r="E127" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E127" s="20"/>
       <c r="F127" s="20"/>
       <c r="G127" s="20"/>
       <c r="H127" s="20"/>
@@ -3209,41 +3230,46 @@
     <row r="128" spans="1:10">
       <c r="A128" s="31"/>
       <c r="B128" s="29"/>
-      <c r="C128" s="6" t="s">
-        <v>73</v>
+      <c r="C128" s="19" t="s">
+        <v>129</v>
       </c>
       <c r="D128" s="20"/>
       <c r="E128" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F128" s="20"/>
       <c r="G128" s="20"/>
       <c r="H128" s="20"/>
       <c r="I128" s="21"/>
-      <c r="J128" s="21"/>
+      <c r="J128" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="129" spans="1:10">
       <c r="A129" s="31"/>
       <c r="B129" s="29"/>
-      <c r="C129" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E129" s="20"/>
+      <c r="C129" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D129" s="20"/>
+      <c r="E129" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F129" s="20"/>
       <c r="G129" s="20"/>
       <c r="H129" s="20"/>
       <c r="I129" s="21"/>
-      <c r="J129" s="21"/>
+      <c r="J129" s="21">
+        <v>3</v>
+      </c>
     </row>
     <row r="130" spans="1:10">
       <c r="A130" s="31"/>
       <c r="B130" s="29"/>
-      <c r="C130" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D130" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C130" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D130" s="20"/>
       <c r="E130" s="20"/>
       <c r="F130" s="20"/>
       <c r="G130" s="20"/>
@@ -3254,45 +3280,47 @@
     <row r="131" spans="1:10">
       <c r="A131" s="31"/>
       <c r="B131" s="29"/>
-      <c r="C131" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D131" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E131" s="20"/>
+      <c r="C131" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D131" s="20"/>
+      <c r="E131" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F131" s="20"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
       <c r="I131" s="21"/>
-      <c r="J131" s="21"/>
+      <c r="J131" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="132" spans="1:10">
       <c r="A132" s="31"/>
       <c r="B132" s="29"/>
       <c r="C132" s="6" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="D132" s="20"/>
       <c r="E132" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F132" s="20"/>
       <c r="G132" s="20"/>
       <c r="H132" s="20"/>
       <c r="I132" s="21"/>
-      <c r="J132" s="21"/>
+      <c r="J132" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="133" spans="1:10">
       <c r="A133" s="31"/>
       <c r="B133" s="29"/>
-      <c r="C133" s="6" t="s">
-        <v>73</v>
+      <c r="C133" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="D133" s="20"/>
-      <c r="E133" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E133" s="20"/>
       <c r="F133" s="20"/>
       <c r="G133" s="20"/>
       <c r="H133" s="20"/>
@@ -3300,62 +3328,68 @@
       <c r="J133" s="21"/>
     </row>
     <row r="134" spans="1:10">
-      <c r="A134" s="30">
-        <v>6</v>
-      </c>
-      <c r="B134" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C134" s="18" t="s">
-        <v>25</v>
+      <c r="A134" s="31"/>
+      <c r="B134" s="29"/>
+      <c r="C134" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="D134" s="20"/>
-      <c r="E134" s="20"/>
+      <c r="E134" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F134" s="20"/>
       <c r="G134" s="20"/>
       <c r="H134" s="20"/>
       <c r="I134" s="21"/>
-      <c r="J134" s="21"/>
+      <c r="J134" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135" s="31"/>
-      <c r="B135" s="34"/>
-      <c r="C135" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D135" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E135" s="20"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D135" s="20"/>
+      <c r="E135" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F135" s="20"/>
       <c r="G135" s="20"/>
       <c r="H135" s="20"/>
       <c r="I135" s="21"/>
-      <c r="J135" s="21"/>
+      <c r="J135" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="136" spans="1:10">
       <c r="A136" s="31"/>
-      <c r="B136" s="34"/>
+      <c r="B136" s="29"/>
       <c r="C136" s="6" t="s">
-        <v>67</v>
+        <v>131</v>
       </c>
       <c r="D136" s="20"/>
       <c r="E136" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F136" s="20"/>
       <c r="G136" s="20"/>
       <c r="H136" s="20"/>
       <c r="I136" s="21"/>
-      <c r="J136" s="21"/>
+      <c r="J136" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="137" spans="1:10">
       <c r="A137" s="31"/>
-      <c r="B137" s="34"/>
-      <c r="C137" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D137" s="20"/>
+      <c r="B137" s="29"/>
+      <c r="C137" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D137" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E137" s="20"/>
       <c r="F137" s="20"/>
       <c r="G137" s="20"/>
@@ -3365,13 +3399,11 @@
     </row>
     <row r="138" spans="1:10">
       <c r="A138" s="31"/>
-      <c r="B138" s="34"/>
-      <c r="C138" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D138" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="B138" s="29"/>
+      <c r="C138" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="20"/>
       <c r="E138" s="20"/>
       <c r="F138" s="20"/>
       <c r="G138" s="20"/>
@@ -3381,12 +3413,12 @@
     </row>
     <row r="139" spans="1:10">
       <c r="A139" s="31"/>
-      <c r="B139" s="34"/>
+      <c r="B139" s="29"/>
       <c r="C139" s="6" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E139" s="20"/>
       <c r="F139" s="20"/>
@@ -3397,11 +3429,13 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140" s="31"/>
-      <c r="B140" s="34"/>
-      <c r="C140" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D140" s="20"/>
+      <c r="B140" s="29"/>
+      <c r="C140" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D140" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E140" s="20"/>
       <c r="F140" s="20"/>
       <c r="G140" s="20"/>
@@ -3411,14 +3445,14 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141" s="31"/>
-      <c r="B141" s="34"/>
+      <c r="B141" s="29"/>
       <c r="C141" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D141" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E141" s="20"/>
+        <v>71</v>
+      </c>
+      <c r="D141" s="20"/>
+      <c r="E141" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F141" s="20"/>
       <c r="G141" s="20"/>
       <c r="H141" s="20"/>
@@ -3427,14 +3461,14 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142" s="31"/>
-      <c r="B142" s="34"/>
+      <c r="B142" s="29"/>
       <c r="C142" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D142" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E142" s="20"/>
+        <v>72</v>
+      </c>
+      <c r="D142" s="20"/>
+      <c r="E142" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="F142" s="20"/>
       <c r="G142" s="20"/>
       <c r="H142" s="20"/>
@@ -3443,13 +3477,11 @@
     </row>
     <row r="143" spans="1:10">
       <c r="A143" s="31"/>
-      <c r="B143" s="34"/>
-      <c r="C143" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D143" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="B143" s="29"/>
+      <c r="C143" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D143" s="20"/>
       <c r="E143" s="20"/>
       <c r="F143" s="20"/>
       <c r="G143" s="20"/>
@@ -3459,11 +3491,13 @@
     </row>
     <row r="144" spans="1:10">
       <c r="A144" s="31"/>
-      <c r="B144" s="34"/>
-      <c r="C144" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D144" s="20"/>
+      <c r="B144" s="29"/>
+      <c r="C144" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D144" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E144" s="20"/>
       <c r="F144" s="20"/>
       <c r="G144" s="20"/>
@@ -3473,14 +3507,14 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" s="31"/>
-      <c r="B145" s="34"/>
+      <c r="B145" s="29"/>
       <c r="C145" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D145" s="20"/>
-      <c r="E145" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D145" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E145" s="20"/>
       <c r="F145" s="20"/>
       <c r="G145" s="20"/>
       <c r="H145" s="20"/>
@@ -3489,13 +3523,13 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146" s="31"/>
-      <c r="B146" s="34"/>
+      <c r="B146" s="29"/>
       <c r="C146" s="6" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D146" s="20"/>
       <c r="E146" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F146" s="20"/>
       <c r="G146" s="20"/>
@@ -3505,13 +3539,13 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147" s="31"/>
-      <c r="B147" s="34"/>
+      <c r="B147" s="29"/>
       <c r="C147" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D147" s="20"/>
       <c r="E147" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F147" s="20"/>
       <c r="G147" s="20"/>
@@ -3520,15 +3554,17 @@
       <c r="J147" s="21"/>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148" s="31"/>
-      <c r="B148" s="34"/>
-      <c r="C148" s="6" t="s">
-        <v>73</v>
+      <c r="A148" s="30">
+        <v>6</v>
+      </c>
+      <c r="B148" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="D148" s="20"/>
-      <c r="E148" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E148" s="20"/>
       <c r="F148" s="20"/>
       <c r="G148" s="20"/>
       <c r="H148" s="20"/>
@@ -3539,12 +3575,12 @@
       <c r="A149" s="31"/>
       <c r="B149" s="34"/>
       <c r="C149" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D149" s="20"/>
-      <c r="E149" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D149" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E149" s="20"/>
       <c r="F149" s="20"/>
       <c r="G149" s="20"/>
       <c r="H149" s="20"/>
@@ -3554,12 +3590,12 @@
     <row r="150" spans="1:10">
       <c r="A150" s="31"/>
       <c r="B150" s="34"/>
-      <c r="C150" s="26" t="s">
-        <v>77</v>
+      <c r="C150" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="D150" s="20"/>
       <c r="E150" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F150" s="20"/>
       <c r="G150" s="20"/>
@@ -3571,7 +3607,7 @@
       <c r="A151" s="31"/>
       <c r="B151" s="34"/>
       <c r="C151" s="18" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D151" s="20"/>
       <c r="E151" s="20"/>
@@ -3585,12 +3621,12 @@
       <c r="A152" s="31"/>
       <c r="B152" s="34"/>
       <c r="C152" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D152" s="20"/>
-      <c r="E152" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D152" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E152" s="20"/>
       <c r="F152" s="20"/>
       <c r="G152" s="20"/>
       <c r="H152" s="20"/>
@@ -3601,12 +3637,12 @@
       <c r="A153" s="31"/>
       <c r="B153" s="34"/>
       <c r="C153" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D153" s="20"/>
-      <c r="E153" s="20" t="s">
-        <v>83</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D153" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E153" s="20"/>
       <c r="F153" s="20"/>
       <c r="G153" s="20"/>
       <c r="H153" s="20"/>
@@ -3616,13 +3652,11 @@
     <row r="154" spans="1:10">
       <c r="A154" s="31"/>
       <c r="B154" s="34"/>
-      <c r="C154" s="6" t="s">
-        <v>62</v>
+      <c r="C154" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="D154" s="20"/>
-      <c r="E154" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="E154" s="20"/>
       <c r="F154" s="20"/>
       <c r="G154" s="20"/>
       <c r="H154" s="20"/>
@@ -3632,13 +3666,13 @@
     <row r="155" spans="1:10">
       <c r="A155" s="31"/>
       <c r="B155" s="34"/>
-      <c r="C155" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D155" s="20"/>
-      <c r="E155" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="C155" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D155" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E155" s="20"/>
       <c r="F155" s="20"/>
       <c r="G155" s="20"/>
       <c r="H155" s="20"/>
@@ -3646,10 +3680,14 @@
       <c r="J155" s="21"/>
     </row>
     <row r="156" spans="1:10">
-      <c r="A156" s="32"/>
-      <c r="B156" s="28"/>
-      <c r="C156" s="18"/>
-      <c r="D156" s="20"/>
+      <c r="A156" s="31"/>
+      <c r="B156" s="34"/>
+      <c r="C156" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D156" s="20" t="s">
+        <v>82</v>
+      </c>
       <c r="E156" s="20"/>
       <c r="F156" s="20"/>
       <c r="G156" s="20"/>
@@ -3658,181 +3696,231 @@
       <c r="J156" s="21"/>
     </row>
     <row r="157" spans="1:10">
-      <c r="A157" s="3"/>
-      <c r="C157" s="3"/>
+      <c r="A157" s="31"/>
+      <c r="B157" s="34"/>
+      <c r="C157" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D157" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E157" s="20"/>
+      <c r="F157" s="20"/>
+      <c r="G157" s="20"/>
+      <c r="H157" s="20"/>
+      <c r="I157" s="21"/>
+      <c r="J157" s="21"/>
     </row>
     <row r="158" spans="1:10">
-      <c r="A158" s="14" t="s">
+      <c r="A158" s="31"/>
+      <c r="B158" s="34"/>
+      <c r="C158" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D158" s="20"/>
+      <c r="E158" s="20"/>
+      <c r="F158" s="20"/>
+      <c r="G158" s="20"/>
+      <c r="H158" s="20"/>
+      <c r="I158" s="21"/>
+      <c r="J158" s="21"/>
+    </row>
+    <row r="159" spans="1:10">
+      <c r="A159" s="31"/>
+      <c r="B159" s="34"/>
+      <c r="C159" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D159" s="20"/>
+      <c r="E159" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F159" s="20"/>
+      <c r="G159" s="20"/>
+      <c r="H159" s="20"/>
+      <c r="I159" s="21"/>
+      <c r="J159" s="21"/>
+    </row>
+    <row r="160" spans="1:10">
+      <c r="A160" s="31"/>
+      <c r="B160" s="34"/>
+      <c r="C160" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D160" s="20"/>
+      <c r="E160" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F160" s="20"/>
+      <c r="G160" s="20"/>
+      <c r="H160" s="20"/>
+      <c r="I160" s="21"/>
+      <c r="J160" s="21"/>
+    </row>
+    <row r="161" spans="1:10">
+      <c r="A161" s="31"/>
+      <c r="B161" s="34"/>
+      <c r="C161" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D161" s="20"/>
+      <c r="E161" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F161" s="20"/>
+      <c r="G161" s="20"/>
+      <c r="H161" s="20"/>
+      <c r="I161" s="21"/>
+      <c r="J161" s="21"/>
+    </row>
+    <row r="162" spans="1:10">
+      <c r="A162" s="31"/>
+      <c r="B162" s="34"/>
+      <c r="C162" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D162" s="20"/>
+      <c r="E162" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F162" s="20"/>
+      <c r="G162" s="20"/>
+      <c r="H162" s="20"/>
+      <c r="I162" s="21"/>
+      <c r="J162" s="21"/>
+    </row>
+    <row r="163" spans="1:10">
+      <c r="A163" s="31"/>
+      <c r="B163" s="34"/>
+      <c r="C163" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D163" s="20"/>
+      <c r="E163" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F163" s="20"/>
+      <c r="G163" s="20"/>
+      <c r="H163" s="20"/>
+      <c r="I163" s="21"/>
+      <c r="J163" s="21"/>
+    </row>
+    <row r="164" spans="1:10">
+      <c r="A164" s="31"/>
+      <c r="B164" s="34"/>
+      <c r="C164" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D164" s="20"/>
+      <c r="E164" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F164" s="20"/>
+      <c r="G164" s="20"/>
+      <c r="H164" s="20"/>
+      <c r="I164" s="21"/>
+      <c r="J164" s="21"/>
+    </row>
+    <row r="165" spans="1:10">
+      <c r="A165" s="31"/>
+      <c r="B165" s="34"/>
+      <c r="C165" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D165" s="20"/>
+      <c r="E165" s="20"/>
+      <c r="F165" s="20"/>
+      <c r="G165" s="20"/>
+      <c r="H165" s="20"/>
+      <c r="I165" s="21"/>
+      <c r="J165" s="21"/>
+    </row>
+    <row r="166" spans="1:10">
+      <c r="A166" s="31"/>
+      <c r="B166" s="34"/>
+      <c r="C166" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D166" s="20"/>
+      <c r="E166" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F166" s="20"/>
+      <c r="G166" s="20"/>
+      <c r="H166" s="20"/>
+      <c r="I166" s="21"/>
+      <c r="J166" s="21"/>
+    </row>
+    <row r="167" spans="1:10">
+      <c r="A167" s="31"/>
+      <c r="B167" s="34"/>
+      <c r="C167" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D167" s="20"/>
+      <c r="E167" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F167" s="20"/>
+      <c r="G167" s="20"/>
+      <c r="H167" s="20"/>
+      <c r="I167" s="21"/>
+      <c r="J167" s="21"/>
+    </row>
+    <row r="168" spans="1:10">
+      <c r="A168" s="31"/>
+      <c r="B168" s="34"/>
+      <c r="C168" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D168" s="20"/>
+      <c r="E168" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F168" s="20"/>
+      <c r="G168" s="20"/>
+      <c r="H168" s="20"/>
+      <c r="I168" s="21"/>
+      <c r="J168" s="21"/>
+    </row>
+    <row r="169" spans="1:10">
+      <c r="A169" s="31"/>
+      <c r="B169" s="34"/>
+      <c r="C169" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D169" s="20"/>
+      <c r="E169" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F169" s="20"/>
+      <c r="G169" s="20"/>
+      <c r="H169" s="20"/>
+      <c r="I169" s="21"/>
+      <c r="J169" s="21"/>
+    </row>
+    <row r="170" spans="1:10">
+      <c r="A170" s="32"/>
+      <c r="B170" s="28"/>
+      <c r="C170" s="18"/>
+      <c r="D170" s="20"/>
+      <c r="E170" s="20"/>
+      <c r="F170" s="20"/>
+      <c r="G170" s="20"/>
+      <c r="H170" s="20"/>
+      <c r="I170" s="21"/>
+      <c r="J170" s="21"/>
+    </row>
+    <row r="171" spans="1:10">
+      <c r="A171" s="3"/>
+      <c r="C171" s="3"/>
+    </row>
+    <row r="172" spans="1:10">
+      <c r="A172" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="3"/>
-      <c r="F158" s="3"/>
-      <c r="G158" s="3"/>
-      <c r="H158" s="3"/>
-      <c r="J158" s="3"/>
-    </row>
-    <row r="159" spans="1:10">
-      <c r="A159" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B159" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D159" s="3"/>
-      <c r="E159" s="3"/>
-      <c r="F159" s="3"/>
-      <c r="G159" s="3"/>
-      <c r="H159" s="3"/>
-      <c r="J159" s="3"/>
-    </row>
-    <row r="160" spans="1:10" ht="60">
-      <c r="A160" s="15">
-        <v>1</v>
-      </c>
-      <c r="B160" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C160" s="4">
-        <v>1</v>
-      </c>
-      <c r="D160" s="3"/>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
-      <c r="G160" s="3"/>
-      <c r="H160" s="3"/>
-      <c r="J160" s="3"/>
-    </row>
-    <row r="161" spans="1:10" ht="30">
-      <c r="A161" s="17">
-        <v>2</v>
-      </c>
-      <c r="B161" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C161" s="17">
-        <v>2</v>
-      </c>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
-      <c r="G161" s="3"/>
-      <c r="H161" s="3"/>
-      <c r="J161" s="3"/>
-    </row>
-    <row r="162" spans="1:10" ht="30">
-      <c r="A162" s="17">
-        <v>3</v>
-      </c>
-      <c r="B162" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C162" s="17">
-        <v>3</v>
-      </c>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
-      <c r="G162" s="3"/>
-      <c r="H162" s="3"/>
-      <c r="J162" s="3"/>
-    </row>
-    <row r="163" spans="1:10" ht="30">
-      <c r="A163" s="17">
-        <v>4</v>
-      </c>
-      <c r="B163" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C163" s="17">
-        <v>4</v>
-      </c>
-      <c r="D163" s="3"/>
-      <c r="E163" s="3"/>
-      <c r="F163" s="3"/>
-      <c r="G163" s="3"/>
-      <c r="H163" s="3"/>
-      <c r="J163" s="3"/>
-    </row>
-    <row r="164" spans="1:10" ht="30">
-      <c r="A164" s="17">
-        <v>5</v>
-      </c>
-      <c r="B164" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C164" s="17">
-        <v>5</v>
-      </c>
-      <c r="D164" s="3"/>
-      <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
-      <c r="G164" s="3"/>
-      <c r="H164" s="3"/>
-      <c r="J164" s="3"/>
-    </row>
-    <row r="165" spans="1:10">
-      <c r="D165" s="3"/>
-      <c r="E165" s="3"/>
-      <c r="F165" s="3"/>
-      <c r="G165" s="3"/>
-      <c r="H165" s="3"/>
-      <c r="J165" s="3"/>
-    </row>
-    <row r="166" spans="1:10">
-      <c r="D166" s="3"/>
-      <c r="E166" s="3"/>
-      <c r="F166" s="3"/>
-      <c r="G166" s="3"/>
-      <c r="H166" s="3"/>
-      <c r="J166" s="3"/>
-    </row>
-    <row r="167" spans="1:10">
-      <c r="D167" s="3"/>
-      <c r="E167" s="3"/>
-      <c r="F167" s="3"/>
-      <c r="G167" s="3"/>
-      <c r="H167" s="3"/>
-      <c r="J167" s="3"/>
-    </row>
-    <row r="168" spans="1:10">
-      <c r="D168" s="3"/>
-      <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3"/>
-      <c r="H168" s="3"/>
-      <c r="J168" s="3"/>
-    </row>
-    <row r="169" spans="1:10">
-      <c r="D169" s="3"/>
-      <c r="E169" s="3"/>
-      <c r="F169" s="3"/>
-      <c r="G169" s="3"/>
-      <c r="H169" s="3"/>
-      <c r="J169" s="3"/>
-    </row>
-    <row r="170" spans="1:10">
-      <c r="D170" s="3"/>
-      <c r="E170" s="3"/>
-      <c r="F170" s="3"/>
-      <c r="G170" s="3"/>
-      <c r="H170" s="3"/>
-      <c r="J170" s="3"/>
-    </row>
-    <row r="171" spans="1:10">
-      <c r="D171" s="3"/>
-      <c r="E171" s="3"/>
-      <c r="F171" s="3"/>
-      <c r="G171" s="3"/>
-      <c r="H171" s="3"/>
-      <c r="J171" s="3"/>
-    </row>
-    <row r="172" spans="1:10">
+      <c r="B172" s="3"/>
+      <c r="C172" s="3"/>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
       <c r="F172" s="3"/>
@@ -3841,6 +3929,15 @@
       <c r="J172" s="3"/>
     </row>
     <row r="173" spans="1:10">
+      <c r="A173" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B173" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
       <c r="F173" s="3"/>
@@ -3848,7 +3945,16 @@
       <c r="H173" s="3"/>
       <c r="J173" s="3"/>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" ht="60">
+      <c r="A174" s="15">
+        <v>1</v>
+      </c>
+      <c r="B174" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C174" s="4">
+        <v>1</v>
+      </c>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
@@ -3856,7 +3962,16 @@
       <c r="H174" s="3"/>
       <c r="J174" s="3"/>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" ht="30">
+      <c r="A175" s="17">
+        <v>2</v>
+      </c>
+      <c r="B175" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C175" s="17">
+        <v>2</v>
+      </c>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
       <c r="F175" s="3"/>
@@ -3864,7 +3979,16 @@
       <c r="H175" s="3"/>
       <c r="J175" s="3"/>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" ht="30">
+      <c r="A176" s="17">
+        <v>3</v>
+      </c>
+      <c r="B176" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C176" s="17">
+        <v>3</v>
+      </c>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
       <c r="F176" s="3"/>
@@ -3872,7 +3996,16 @@
       <c r="H176" s="3"/>
       <c r="J176" s="3"/>
     </row>
-    <row r="177" spans="4:10">
+    <row r="177" spans="1:10" ht="30">
+      <c r="A177" s="17">
+        <v>4</v>
+      </c>
+      <c r="B177" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C177" s="17">
+        <v>4</v>
+      </c>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
@@ -3880,7 +4013,16 @@
       <c r="H177" s="3"/>
       <c r="J177" s="3"/>
     </row>
-    <row r="178" spans="4:10">
+    <row r="178" spans="1:10" ht="30">
+      <c r="A178" s="17">
+        <v>5</v>
+      </c>
+      <c r="B178" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C178" s="17">
+        <v>5</v>
+      </c>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
       <c r="F178" s="3"/>
@@ -3888,7 +4030,7 @@
       <c r="H178" s="3"/>
       <c r="J178" s="3"/>
     </row>
-    <row r="179" spans="4:10">
+    <row r="179" spans="1:10">
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
@@ -3896,23 +4038,135 @@
       <c r="H179" s="3"/>
       <c r="J179" s="3"/>
     </row>
+    <row r="180" spans="1:10">
+      <c r="D180" s="3"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="3"/>
+      <c r="G180" s="3"/>
+      <c r="H180" s="3"/>
+      <c r="J180" s="3"/>
+    </row>
+    <row r="181" spans="1:10">
+      <c r="D181" s="3"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
+      <c r="H181" s="3"/>
+      <c r="J181" s="3"/>
+    </row>
+    <row r="182" spans="1:10">
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="3"/>
+      <c r="G182" s="3"/>
+      <c r="H182" s="3"/>
+      <c r="J182" s="3"/>
+    </row>
+    <row r="183" spans="1:10">
+      <c r="D183" s="3"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="3"/>
+      <c r="J183" s="3"/>
+    </row>
+    <row r="184" spans="1:10">
+      <c r="D184" s="3"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="3"/>
+      <c r="J184" s="3"/>
+    </row>
+    <row r="185" spans="1:10">
+      <c r="D185" s="3"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="3"/>
+      <c r="G185" s="3"/>
+      <c r="H185" s="3"/>
+      <c r="J185" s="3"/>
+    </row>
+    <row r="186" spans="1:10">
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="3"/>
+      <c r="J186" s="3"/>
+    </row>
+    <row r="187" spans="1:10">
+      <c r="D187" s="3"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
+      <c r="J187" s="3"/>
+    </row>
+    <row r="188" spans="1:10">
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="3"/>
+      <c r="J188" s="3"/>
+    </row>
+    <row r="189" spans="1:10">
+      <c r="D189" s="3"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3"/>
+      <c r="J189" s="3"/>
+    </row>
+    <row r="190" spans="1:10">
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="3"/>
+      <c r="J190" s="3"/>
+    </row>
+    <row r="191" spans="1:10">
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="3"/>
+      <c r="J191" s="3"/>
+    </row>
+    <row r="192" spans="1:10">
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="3"/>
+      <c r="J192" s="3"/>
+    </row>
+    <row r="193" spans="4:10">
+      <c r="D193" s="3"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
+      <c r="G193" s="3"/>
+      <c r="H193" s="3"/>
+      <c r="J193" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A134:A156"/>
-    <mergeCell ref="B134:B156"/>
-    <mergeCell ref="B54:B133"/>
-    <mergeCell ref="A54:A133"/>
-    <mergeCell ref="B29:B53"/>
-    <mergeCell ref="A29:A53"/>
+    <mergeCell ref="A148:A170"/>
+    <mergeCell ref="B148:B170"/>
+    <mergeCell ref="B62:B147"/>
+    <mergeCell ref="A62:A147"/>
+    <mergeCell ref="B37:B61"/>
+    <mergeCell ref="A37:A61"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B28"/>
-    <mergeCell ref="A12:A28"/>
+    <mergeCell ref="B12:B36"/>
+    <mergeCell ref="A12:A36"/>
     <mergeCell ref="A8:A11"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D18 D2:H15 F16:H18 D22 D19:H21 F22:H22 D26 F26:H26 D23:H25 D92:D128 D130:D177 F92:H177 E132:E177 D27:H91 E93:E130">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D22 D2:H15 F16:H22 D30 D23:H29 F30:H30 D34 F34:H34 D31:H33 D106:D142 D144:D191 F106:H191 E146:E191 E107:E144 D35:H105 E21">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>